<commit_message>
Update Health Care Sys Sprint 5 (Iteration 4)  Backlog Burndown.xlsx
Added my actual worked hours
</commit_message>
<xml_diff>
--- a/Documents/Health Care Sys Sprint 5 (Iteration 4)  Backlog Burndown.xlsx
+++ b/Documents/Health Care Sys Sprint 5 (Iteration 4)  Backlog Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jabes\Downloads\HealthCareSync\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787A4CD1-624C-4190-98BB-B83AD214CC0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4502CF-291B-44BA-98E2-A6CF7F881D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -694,7 +694,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1741,8 +1741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1893,9 +1893,15 @@
       <c r="E7" s="13">
         <v>8</v>
       </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
+      <c r="F7" s="19">
+        <v>0</v>
+      </c>
+      <c r="G7" s="19">
+        <v>0</v>
+      </c>
+      <c r="H7" s="19">
+        <v>7</v>
+      </c>
       <c r="I7" s="19"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -1965,7 +1971,7 @@
       </c>
       <c r="H13" s="16">
         <f>SUM(H3:H12)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I13" s="16">
         <f>SUM(I3:I12)</f>
@@ -1995,6 +2001,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010041FBA4D6976FF34697CED57BA3121E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="90eba6b134f98a2dcd6f2554d0702a0d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7" xmlns:ns4="3bea4f68-df9b-425b-8be9-897e521449f8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b10b116c70102c4d21148cc2133431f" ns3:_="" ns4:_="">
     <xsd:import namespace="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7"/>
@@ -2241,15 +2256,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2257,6 +2263,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C61A29E-1F26-4720-A5C6-A54EFA5CA6A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2271,14 +2285,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updated sprint backlog for the last iteration
</commit_message>
<xml_diff>
--- a/Documents/Health Care Sys Sprint 5 (Iteration 4)  Backlog Burndown.xlsx
+++ b/Documents/Health Care Sys Sprint 5 (Iteration 4)  Backlog Burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Ahmad\HealthCareSync\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0CF000-307D-48CF-AA3D-575F79273866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27321FB3-50F7-4365-BF92-D86747D17AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="2235" windowWidth="16380" windowHeight="18030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2610" yWindow="2250" windowWidth="16380" windowHeight="18030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Related User Story</t>
   </si>
@@ -68,351 +68,66 @@
     <t>Estimate</t>
   </si>
   <si>
-    <t>Enter initial diagnosis and order tests for a visit</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Before the user confirms the tests ordered, the user can remove or add more tests to the order. Note that initial diagnosis is optional at the routine checkup stage. The nurse can fill in it later after the doctor exams the patient. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Design UI </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Add functionality to enter intial diagnosis and order tests</t>
-    </r>
-  </si>
-  <si>
-    <t>Enter Test results</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Design UI </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Add functionality to be able to enter test results</t>
-    </r>
-  </si>
-  <si>
-    <t>Enter final diagnosis</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Once the final diagnosis is entered, patient visit information such as the checkup, tests, and diagnosis is read-only. Make sure to prompt the user about it for confirmation. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Design UI </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Add functionality to be able to enter final diagnosis</t>
-    </r>
-  </si>
-  <si>
-    <t>Search patients and view patients' visit information</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Search patients and view patients' visit information (e.g checkup info., tests ordered and/or performed including time, diagnoses, etc. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">2. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Design UI </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Add functionality to search and view patients' visit information</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> admin edit nurse (including updating nurse's password), delete nurse (if there is no visit associated with the nurse, otherwise, deactivate the nurse) </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Design UI </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Add functionality to edit nurse and delete/deactivate nurse</t>
-    </r>
-  </si>
-  <si>
-    <t>Admin edit/delete/deactivate nurse</t>
-  </si>
-  <si>
     <t>Assignees</t>
   </si>
   <si>
     <t xml:space="preserve">Initial </t>
   </si>
   <si>
-    <t>ITERATION 4 DESCRIPTION NOTES:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">note that please be concious about the user-friendlines of your program. It's not user-friendly if the user only sees ids without any detailed information.  It's important that on all the views, it should be clear about
-    the patient's name, dob
-    doctor's name
-    nurse's name
-Each team member must use at least one stored procedure for one of the DB operations for this iteration so that everyone may practice writing stored procedures and see how it helps you reduce the coupling of the SQL statement that would otherwise have been embedded in your code. Please have the stored procedures in the readme.txt file for easy access during the demo. </t>
-  </si>
-  <si>
     <t>Ahmad</t>
   </si>
   <si>
-    <t>Rahman</t>
-  </si>
-  <si>
-    <t>Jabesi</t>
-  </si>
-  <si>
-    <t>Ahmad/Rahman</t>
+    <t>Enter Test Result</t>
+  </si>
+  <si>
+    <t>1. Design UI 2. Add functionality to be able to enter test results</t>
+  </si>
+  <si>
+    <t>Store hashed passwords in the DB</t>
+  </si>
+  <si>
+    <t>1. Add functionality to store hashed passwords for users in the DB (you may use any hashing mechanism --make sure to cite and credit the sources in comments)</t>
+  </si>
+  <si>
+    <t>Admin query requests</t>
+  </si>
+  <si>
+    <t>1. Design UI 2. Add functionality so that the administrator can pose queries in SQL and view the result in tabular format.</t>
+  </si>
+  <si>
+    <t>Admin date reports</t>
+  </si>
+  <si>
+    <t>1. Design UI 2. Add functionality so that the administrator should be able to select any two dates and view a report containing the information about all the visits during the time specified. The visit information should include the visit date, patient id, name, the
+names of the doctor and nurse involved, the tests ordered, test perform date, tests result abnormality, and diagnosis. The result should be sorted by the visit date followed by the last name of the patient</t>
+  </si>
+  <si>
+    <t>Fix where screen is cut off on some machines and others its not</t>
+  </si>
+  <si>
+    <t>BUGS ON UI</t>
+  </si>
+  <si>
+    <t>DEMO NOTES REVISIONS</t>
+  </si>
+  <si>
+    <t>manage_visit page:  -should use case-insensitive search on the visit page, temp needs to have decimal points,**nurse should be loaded automatically
+**error messages for routine checkup are not showing.-
+**better to move format information for visit below the visit label
+- tests are ordered one by one --need to be order several tests together
+- should allow tests to be ordered anytime (remove the 15-min interval limit)</t>
+  </si>
+  <si>
+    <t>manage_appointments page: - error message on the appt time needs to be cleared, - search appointment needs to be clear about it's search by patient name
+- need to make the create appointment and search appointment page more clear so that user knows what to do</t>
+  </si>
+  <si>
+    <t>admin:  -should make nurse's name editable
+- MD created a sp, but not called in the program
+- need to put candeletenurse and delete nurse in one transaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - inactive nurse should not be able to login</t>
   </si>
 </sst>
 </file>
@@ -436,7 +151,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -479,6 +194,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -492,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -506,15 +227,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -568,6 +280,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -691,13 +406,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1742,48 +1457,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="50.42578125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="34.7109375" style="15" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="18" customWidth="1"/>
-    <col min="6" max="9" width="9.140625" style="15"/>
+    <col min="2" max="2" width="50.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="15" customWidth="1"/>
+    <col min="6" max="9" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="24"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="21"/>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1791,222 +1506,206 @@
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="13">
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="10">
         <v>1</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="13">
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+    </row>
+    <row r="4" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="10">
+        <v>1</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+    </row>
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="10">
+        <v>1</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="10">
+        <v>16</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+    </row>
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="10">
+        <v>1</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="10">
         <v>14</v>
       </c>
-      <c r="F3" s="19">
-        <v>14</v>
-      </c>
-      <c r="G3" s="19">
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+    </row>
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="10">
         <v>0</v>
       </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
     </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+    <row r="8" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="13">
-        <v>1</v>
-      </c>
-      <c r="D4" s="13" t="s">
+      <c r="E8" s="4">
+        <v>6</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+    </row>
+    <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-    </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="13">
-        <v>1</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="13">
-        <v>14</v>
-      </c>
-      <c r="F5" s="19">
-        <v>14</v>
-      </c>
-      <c r="G5" s="19">
+      <c r="C9" s="4">
         <v>0</v>
       </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-    </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="13">
-        <v>2</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="13">
-        <v>2</v>
-      </c>
-      <c r="F6" s="19">
-        <v>2</v>
-      </c>
-      <c r="G6" s="19">
-        <v>0</v>
-      </c>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-    </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="13">
-        <v>1</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="13">
-        <v>8</v>
-      </c>
-      <c r="F7" s="19">
-        <v>0</v>
-      </c>
-      <c r="G7" s="19">
-        <v>0</v>
-      </c>
-      <c r="H7" s="19">
-        <v>7</v>
-      </c>
-      <c r="I7" s="19"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="5"/>
-      <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="4"/>
+      <c r="B10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="4"/>
+      <c r="B11" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="7"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="16">
+      <c r="B13" s="19"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="13">
         <f>SUM(F3:F12)</f>
-        <v>30</v>
-      </c>
-      <c r="G13" s="16">
+        <v>0</v>
+      </c>
+      <c r="G13" s="13">
         <f>SUM(G3:G12)</f>
         <v>0</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="13">
         <f>SUM(H3:H12)</f>
-        <v>7</v>
-      </c>
-      <c r="I13" s="16">
+        <v>0</v>
+      </c>
+      <c r="I13" s="13">
         <f>SUM(I3:I12)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="270" x14ac:dyDescent="0.25">
-      <c r="B15" s="22" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2022,6 +1721,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010041FBA4D6976FF34697CED57BA3121E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="90eba6b134f98a2dcd6f2554d0702a0d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7" xmlns:ns4="3bea4f68-df9b-425b-8be9-897e521449f8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b10b116c70102c4d21148cc2133431f" ns3:_="" ns4:_="">
     <xsd:import namespace="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7"/>
@@ -2268,15 +1976,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2284,6 +1983,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C61A29E-1F26-4720-A5C6-A54EFA5CA6A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2298,14 +2005,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fixed all demo notes revisions for the manage visits page
</commit_message>
<xml_diff>
--- a/Documents/Health Care Sys Sprint 5 (Iteration 4)  Backlog Burndown.xlsx
+++ b/Documents/Health Care Sys Sprint 5 (Iteration 4)  Backlog Burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Ahmad\HealthCareSync\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27321FB3-50F7-4365-BF92-D86747D17AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCA2893-D551-4EB3-B13F-5DB8422C7F0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2610" yWindow="2250" windowWidth="16380" windowHeight="18030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23145" yWindow="0" windowWidth="15255" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -272,6 +272,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -280,9 +283,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1460,7 +1460,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1474,10 +1474,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1489,16 +1489,16 @@
       <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
     </row>
     <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="21"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1628,7 +1628,9 @@
       <c r="E8" s="4">
         <v>6</v>
       </c>
-      <c r="F8" s="18"/>
+      <c r="F8" s="18">
+        <v>0</v>
+      </c>
       <c r="G8" s="18"/>
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
@@ -1664,7 +1666,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="20" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="4">
@@ -1721,15 +1723,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010041FBA4D6976FF34697CED57BA3121E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="90eba6b134f98a2dcd6f2554d0702a0d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7" xmlns:ns4="3bea4f68-df9b-425b-8be9-897e521449f8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b10b116c70102c4d21148cc2133431f" ns3:_="" ns4:_="">
     <xsd:import namespace="c53cb6ec-2191-4daf-a6fa-9a7ffd5e80d7"/>
@@ -1976,6 +1969,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1983,14 +1985,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C61A29E-1F26-4720-A5C6-A54EFA5CA6A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2005,6 +1999,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3EC1687-D4A5-4FCD-9DED-ECE2599FA11D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>